<commit_message>
v1 release: Updated database, added checkout script, added fully functioning qty/stock mechanism, added local storage feature, added AR guidance scene, fixed checkout scene (still no scrollable)
</commit_message>
<xml_diff>
--- a/Assets/Firebase/Database Mapping.xlsx
+++ b/Assets/Firebase/Database Mapping.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="19815" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="category" sheetId="1" r:id="rId1"/>
     <sheet name="item" sheetId="2" r:id="rId2"/>
     <sheet name="kabupaten" sheetId="3" r:id="rId3"/>
+    <sheet name="users" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">item!$A$1:$C$44</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="165">
   <si>
     <t>code</t>
   </si>
@@ -493,6 +494,27 @@
   </si>
   <si>
     <t>{'code': '15','name': 'KOTA METRO'},</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin@example.com</t>
+  </si>
+  <si>
+    <t>adminadmin</t>
+  </si>
+  <si>
+    <t>{'username': 'admin','email': 'admin@example.com','password': 'adminadmin'},</t>
   </si>
 </sst>
 </file>
@@ -500,21 +522,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -529,17 +545,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -558,9 +565,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -572,18 +609,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -596,7 +626,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -611,39 +649,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -657,8 +671,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -673,7 +695,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,7 +725,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,25 +809,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -727,133 +869,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,17 +889,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -897,15 +937,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -921,26 +952,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -955,170 +986,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1651,13 +1676,13 @@
   <sheetPr/>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+    <sheetView topLeftCell="B5" workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="48.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.2857142857143" style="2" customWidth="1"/>
     <col min="4" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="21.4285714285714" customWidth="1"/>
     <col min="7" max="7" width="79.1428571428571" customWidth="1"/>
@@ -1667,7 +1692,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1693,16 +1718,16 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F2" t="str">
@@ -1721,16 +1746,16 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F3" t="str">
@@ -1749,16 +1774,16 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F4" t="str">
@@ -1777,16 +1802,16 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F5" t="str">
@@ -1805,16 +1830,16 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F6" t="str">
@@ -1833,16 +1858,16 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F7" t="str">
@@ -1861,16 +1886,16 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F8" t="str">
@@ -1889,16 +1914,16 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F9" t="str">
@@ -1917,16 +1942,16 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>5</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F10" t="str">
@@ -1945,16 +1970,16 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F11" t="str">
@@ -1973,16 +1998,16 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>5</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F12" t="str">
@@ -2001,16 +2026,16 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F13" t="str">
@@ -2029,16 +2054,16 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>11</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F14" t="str">
@@ -2057,16 +2082,16 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>2</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F15" t="str">
@@ -2085,16 +2110,16 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <v>3</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F16" t="str">
@@ -2113,16 +2138,16 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="4">
         <v>3</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F17" t="str">
@@ -2141,16 +2166,16 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="4">
         <v>3</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F18" t="str">
@@ -2169,16 +2194,16 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="4">
         <v>3</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F19" t="str">
@@ -2197,16 +2222,16 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="4">
         <v>3</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F20" t="str">
@@ -2225,16 +2250,16 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="4">
         <v>3</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F21" t="str">
@@ -2253,16 +2278,16 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="4">
         <v>4</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F22" t="str">
@@ -2281,16 +2306,16 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="4">
         <v>4</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F23" t="str">
@@ -2309,16 +2334,16 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="4">
         <v>4</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F24" t="str">
@@ -2337,16 +2362,16 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="4">
         <v>11</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F25" t="str">
@@ -2365,16 +2390,16 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="4">
         <v>6</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F26" t="str">
@@ -2393,16 +2418,16 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="4">
         <v>6</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F27" t="str">
@@ -2421,16 +2446,16 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="4">
         <v>6</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F28" t="str">
@@ -2449,16 +2474,16 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="4">
         <v>7</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F29" t="str">
@@ -2477,16 +2502,16 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="4">
         <v>8</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F30" t="str">
@@ -2505,16 +2530,16 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="4">
         <v>8</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F31" t="str">
@@ -2533,16 +2558,16 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="4">
         <v>8</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F32" t="str">
@@ -2561,16 +2586,16 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="4">
         <v>2</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F33" t="str">
@@ -2589,16 +2614,16 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="4">
         <v>11</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F34" t="str">
@@ -2617,16 +2642,16 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="4">
         <v>11</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F35" t="str">
@@ -2645,16 +2670,16 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="4">
         <v>9</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F36" t="str">
@@ -2673,16 +2698,16 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="4">
         <v>9</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F37" t="str">
@@ -2701,16 +2726,16 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="4">
         <v>9</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F38" t="str">
@@ -2729,16 +2754,16 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="4">
         <v>9</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F39" t="str">
@@ -2757,16 +2782,16 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="4">
         <v>9</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F40" t="str">
@@ -2785,16 +2810,16 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="4">
         <v>10</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F41" t="str">
@@ -2813,16 +2838,16 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="4">
         <v>10</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F42" t="str">
@@ -2841,16 +2866,16 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="4">
         <v>11</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F43" t="str">
@@ -2869,16 +2894,16 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="4">
         <v>11</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F44" t="str">
@@ -3160,4 +3185,65 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="10.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="27.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="19.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="79" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"{'"&amp;$A$1&amp;"': '"&amp;A2&amp;"','"&amp;$B$1&amp;"': '"&amp;B2&amp;"','"&amp;$C$1&amp;"': '"&amp;C2&amp;"'},"</f>
+        <v>{'username': 'admin','email': 'admin@example.com','password': 'adminadmin'},</v>
+      </c>
+      <c r="E2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="admin@example.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>